<commit_message>
20190423 update test data
</commit_message>
<xml_diff>
--- a/data/tcData.xlsx
+++ b/data/tcData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>username</t>
   </si>
@@ -106,79 +106,82 @@
     <t>test发送邮件1</t>
   </si>
   <si>
+    <t>发送普通测试邮件</t>
+  </si>
+  <si>
+    <t>test发送邮件2</t>
+  </si>
+  <si>
+    <t>发送带附件的邮件</t>
+  </si>
+  <si>
+    <t>D:\KeyWordDriverTestFrameWork\geckodriver.log</t>
+  </si>
+  <si>
+    <t>linux3</t>
+  </si>
+  <si>
+    <t>1@qq.com</t>
+  </si>
+  <si>
+    <t>添加联系人3</t>
+  </si>
+  <si>
+    <t>linux4</t>
+  </si>
+  <si>
+    <t>1@.com</t>
+  </si>
+  <si>
+    <t>添加联系人4</t>
+  </si>
+  <si>
+    <t>linux5</t>
+  </si>
+  <si>
+    <t>@@qq.cn</t>
+  </si>
+  <si>
+    <t>添加联系人5</t>
+  </si>
+  <si>
+    <t>linux6</t>
+  </si>
+  <si>
+    <t>1@aa.com</t>
+  </si>
+  <si>
+    <t>添加联系人6</t>
+  </si>
+  <si>
+    <t>linux7</t>
+  </si>
+  <si>
+    <t>添加联系人7</t>
+  </si>
+  <si>
+    <t>281754042@qq.com</t>
+  </si>
+  <si>
+    <t>添加联系人8</t>
+  </si>
+  <si>
+    <t>linux9</t>
+  </si>
+  <si>
+    <t>添加联系人9</t>
+  </si>
+  <si>
+    <t>linux10</t>
+  </si>
+  <si>
+    <t>281754044@qq.com</t>
+  </si>
+  <si>
+    <t>添加联系人10</t>
+  </si>
+  <si>
     <t>发送不带附件的邮件</t>
-  </si>
-  <si>
-    <t>test发送邮件2</t>
-  </si>
-  <si>
-    <t>发送带附件的邮件</t>
-  </si>
-  <si>
-    <t>D:\KeyWordDriverTestFrameWork\geckodriver.log</t>
-  </si>
-  <si>
-    <t>linux3</t>
-  </si>
-  <si>
-    <t>1@qq.com</t>
-  </si>
-  <si>
-    <t>添加联系人3</t>
-  </si>
-  <si>
-    <t>linux4</t>
-  </si>
-  <si>
-    <t>1@.com</t>
-  </si>
-  <si>
-    <t>添加联系人4</t>
-  </si>
-  <si>
-    <t>linux5</t>
-  </si>
-  <si>
-    <t>@@qq.cn</t>
-  </si>
-  <si>
-    <t>添加联系人5</t>
-  </si>
-  <si>
-    <t>linux6</t>
-  </si>
-  <si>
-    <t>1@aa.com</t>
-  </si>
-  <si>
-    <t>添加联系人6</t>
-  </si>
-  <si>
-    <t>linux7</t>
-  </si>
-  <si>
-    <t>添加联系人7</t>
-  </si>
-  <si>
-    <t>281754042@qq.com</t>
-  </si>
-  <si>
-    <t>添加联系人8</t>
-  </si>
-  <si>
-    <t>linux9</t>
-  </si>
-  <si>
-    <t>添加联系人9</t>
-  </si>
-  <si>
-    <t>linux10</t>
-  </si>
-  <si>
-    <t>281754044@qq.com</t>
-  </si>
-  <si>
-    <t>添加联系人10</t>
   </si>
 </sst>
 </file>
@@ -237,6 +240,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -244,6 +262,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
@@ -253,7 +286,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -283,8 +345,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -298,79 +361,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -383,187 +386,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,56 +591,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -666,15 +619,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -689,6 +633,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -697,10 +700,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -709,133 +712,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1380,7 +1383,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="3"/>
@@ -1642,7 +1645,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1"/>
     </row>

</xml_diff>